<commit_message>
Migliorata funzione di wordcloud
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -486,25 +486,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>frozenset({'march'})</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>frozenset({'2021'})</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>frozenset({'march'})</t>
-        </is>
-      </c>
       <c r="D2" t="n">
+        <v>0.03314735805710535</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.02297341647522153</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.03314735805710535</v>
       </c>
       <c r="F2" t="n">
         <v>0.01115851657367903</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4857142857142857</v>
+        <v>0.3366336633663366</v>
       </c>
       <c r="H2" t="n">
         <v>14.65318246110325</v>
@@ -513,7 +513,7 @@
         <v>0.01039700851197986</v>
       </c>
       <c r="J2" t="n">
-        <v>1.879991248222295</v>
+        <v>1.4728311184478</v>
       </c>
     </row>
     <row r="3">
@@ -522,25 +522,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>frozenset({'2021'})</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>frozenset({'march'})</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>frozenset({'2021'})</t>
-        </is>
-      </c>
       <c r="D3" t="n">
+        <v>0.02297341647522153</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.03314735805710535</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.02297341647522153</v>
       </c>
       <c r="F3" t="n">
         <v>0.01115851657367903</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3366336633663366</v>
+        <v>0.4857142857142857</v>
       </c>
       <c r="H3" t="n">
         <v>14.65318246110325</v>
@@ -549,7 +549,7 @@
         <v>0.01039700851197986</v>
       </c>
       <c r="J3" t="n">
-        <v>1.4728311184478</v>
+        <v>1.879991248222295</v>
       </c>
     </row>
     <row r="4">
@@ -774,34 +774,34 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>frozenset({'case'})</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>frozenset({'new'})</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>frozenset({'case'})</t>
-        </is>
-      </c>
       <c r="D10" t="n">
+        <v>0.05874630784378077</v>
+      </c>
+      <c r="E10" t="n">
         <v>0.0653101411224155</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.05874630784378077</v>
       </c>
       <c r="F10" t="n">
         <v>0.02067607482769938</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3165829145728643</v>
+        <v>0.3519553072625698</v>
       </c>
       <c r="H10" t="n">
-        <v>5.388984026276635</v>
+        <v>5.388984026276634</v>
       </c>
       <c r="I10" t="n">
         <v>0.01683934517200119</v>
       </c>
       <c r="J10" t="n">
-        <v>1.377275623081527</v>
+        <v>1.44232314430248</v>
       </c>
     </row>
     <row r="11">
@@ -810,34 +810,34 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>frozenset({'new'})</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>frozenset({'case'})</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>frozenset({'new'})</t>
-        </is>
-      </c>
       <c r="D11" t="n">
+        <v>0.0653101411224155</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.05874630784378077</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.0653101411224155</v>
       </c>
       <c r="F11" t="n">
         <v>0.02067607482769938</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3519553072625698</v>
+        <v>0.3165829145728643</v>
       </c>
       <c r="H11" t="n">
-        <v>5.388984026276634</v>
+        <v>5.388984026276635</v>
       </c>
       <c r="I11" t="n">
         <v>0.01683934517200119</v>
       </c>
       <c r="J11" t="n">
-        <v>1.44232314430248</v>
+        <v>1.377275623081527</v>
       </c>
     </row>
     <row r="12">
@@ -1818,25 +1818,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>frozenset({'senat'})</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>frozenset({'relief'})</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>frozenset({'senat'})</t>
-        </is>
-      </c>
       <c r="D39" t="n">
+        <v>0.02067607482769938</v>
+      </c>
+      <c r="E39" t="n">
         <v>0.02888086642599278</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0.02067607482769938</v>
       </c>
       <c r="F39" t="n">
         <v>0.01148670823761076</v>
       </c>
       <c r="G39" t="n">
-        <v>0.3977272727272727</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="H39" t="n">
         <v>19.23611111111111</v>
@@ -1845,7 +1845,7 @@
         <v>0.01088956528229815</v>
       </c>
       <c r="J39" t="n">
-        <v>1.626047271984197</v>
+        <v>2.185018050541517</v>
       </c>
     </row>
     <row r="40">
@@ -1854,25 +1854,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>frozenset({'relief'})</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>frozenset({'senat'})</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>frozenset({'relief'})</t>
-        </is>
-      </c>
       <c r="D40" t="n">
+        <v>0.02888086642599278</v>
+      </c>
+      <c r="E40" t="n">
         <v>0.02067607482769938</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0.02888086642599278</v>
       </c>
       <c r="F40" t="n">
         <v>0.01148670823761076</v>
       </c>
       <c r="G40" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.3977272727272727</v>
       </c>
       <c r="H40" t="n">
         <v>19.23611111111111</v>
@@ -1881,7 +1881,7 @@
         <v>0.01088956528229815</v>
       </c>
       <c r="J40" t="n">
-        <v>2.185018050541517</v>
+        <v>1.626047271984197</v>
       </c>
     </row>
     <row r="41">
@@ -2034,34 +2034,34 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>frozenset({'senat'})</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>frozenset({'trillion'})</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>frozenset({'senat'})</t>
-        </is>
-      </c>
       <c r="D45" t="n">
+        <v>0.02067607482769938</v>
+      </c>
+      <c r="E45" t="n">
         <v>0.01017394158188382</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.02067607482769938</v>
       </c>
       <c r="F45" t="n">
         <v>0.006563833278634723</v>
       </c>
       <c r="G45" t="n">
-        <v>0.6451612903225807</v>
+        <v>0.3174603174603174</v>
       </c>
       <c r="H45" t="n">
-        <v>31.20327700972863</v>
+        <v>31.20327700972862</v>
       </c>
       <c r="I45" t="n">
         <v>0.006353476101195051</v>
       </c>
       <c r="J45" t="n">
-        <v>2.75991288003103</v>
+        <v>1.450210271635845</v>
       </c>
     </row>
     <row r="46">
@@ -2070,34 +2070,34 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>frozenset({'trillion'})</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>frozenset({'senat'})</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>frozenset({'trillion'})</t>
-        </is>
-      </c>
       <c r="D46" t="n">
+        <v>0.01017394158188382</v>
+      </c>
+      <c r="E46" t="n">
         <v>0.02067607482769938</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0.01017394158188382</v>
       </c>
       <c r="F46" t="n">
         <v>0.006563833278634723</v>
       </c>
       <c r="G46" t="n">
-        <v>0.3174603174603174</v>
+        <v>0.6451612903225807</v>
       </c>
       <c r="H46" t="n">
-        <v>31.20327700972862</v>
+        <v>31.20327700972863</v>
       </c>
       <c r="I46" t="n">
         <v>0.006353476101195051</v>
       </c>
       <c r="J46" t="n">
-        <v>1.450210271635845</v>
+        <v>2.75991288003103</v>
       </c>
     </row>
     <row r="47">
@@ -2178,34 +2178,34 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>frozenset({'new', 'death'})</t>
+          <t>frozenset({'case', 'death'})</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>frozenset({'case'})</t>
+          <t>frozenset({'new'})</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.009517558254020347</v>
+        <v>0.01444043321299639</v>
       </c>
       <c r="E49" t="n">
-        <v>0.05874630784378077</v>
+        <v>0.0653101411224155</v>
       </c>
       <c r="F49" t="n">
         <v>0.006235641614702987</v>
       </c>
       <c r="G49" t="n">
-        <v>0.6551724137931035</v>
+        <v>0.4318181818181818</v>
       </c>
       <c r="H49" t="n">
-        <v>11.15257175881333</v>
+        <v>6.61180904522613</v>
       </c>
       <c r="I49" t="n">
-        <v>0.005676520207591191</v>
+        <v>0.005292534883693376</v>
       </c>
       <c r="J49" t="n">
-        <v>2.729635707253037</v>
+        <v>1.645054151624549</v>
       </c>
     </row>
     <row r="50">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>frozenset({'new', 'case'})</t>
+          <t>frozenset({'case', 'new'})</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2250,34 +2250,34 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>frozenset({'death', 'case'})</t>
+          <t>frozenset({'death', 'new'})</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>frozenset({'new'})</t>
+          <t>frozenset({'case'})</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.01444043321299639</v>
+        <v>0.009517558254020347</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0653101411224155</v>
+        <v>0.05874630784378077</v>
       </c>
       <c r="F51" t="n">
         <v>0.006235641614702987</v>
       </c>
       <c r="G51" t="n">
-        <v>0.4318181818181818</v>
+        <v>0.6551724137931035</v>
       </c>
       <c r="H51" t="n">
-        <v>6.61180904522613</v>
+        <v>11.15257175881333</v>
       </c>
       <c r="I51" t="n">
-        <v>0.005292534883693376</v>
+        <v>0.005676520207591191</v>
       </c>
       <c r="J51" t="n">
-        <v>1.645054151624549</v>
+        <v>2.729635707253037</v>
       </c>
     </row>
     <row r="52">
@@ -2286,34 +2286,34 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>frozenset({'new', 'report'})</t>
+          <t>frozenset({'case', 'report'})</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>frozenset({'case'})</t>
+          <t>frozenset({'new'})</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.008861174926156876</v>
+        <v>0.01247128322940597</v>
       </c>
       <c r="E52" t="n">
-        <v>0.05874630784378077</v>
+        <v>0.0653101411224155</v>
       </c>
       <c r="F52" t="n">
         <v>0.006563833278634723</v>
       </c>
       <c r="G52" t="n">
-        <v>0.7407407407407407</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="H52" t="n">
-        <v>12.60914545830747</v>
+        <v>8.058714625760381</v>
       </c>
       <c r="I52" t="n">
-        <v>0.00604327196856512</v>
+        <v>0.005749332010944605</v>
       </c>
       <c r="J52" t="n">
-        <v>3.630549955459702</v>
+        <v>1.973234146519345</v>
       </c>
     </row>
     <row r="53">
@@ -2322,7 +2322,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>frozenset({'new', 'case'})</t>
+          <t>frozenset({'case', 'new'})</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2358,34 +2358,34 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>frozenset({'report', 'case'})</t>
+          <t>frozenset({'report', 'new'})</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>frozenset({'new'})</t>
+          <t>frozenset({'case'})</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.01247128322940597</v>
+        <v>0.008861174926156876</v>
       </c>
       <c r="E54" t="n">
-        <v>0.0653101411224155</v>
+        <v>0.05874630784378077</v>
       </c>
       <c r="F54" t="n">
         <v>0.006563833278634723</v>
       </c>
       <c r="G54" t="n">
-        <v>0.5263157894736842</v>
+        <v>0.7407407407407407</v>
       </c>
       <c r="H54" t="n">
-        <v>8.058714625760381</v>
+        <v>12.60914545830747</v>
       </c>
       <c r="I54" t="n">
-        <v>0.005749332010944605</v>
+        <v>0.00604327196856512</v>
       </c>
       <c r="J54" t="n">
-        <v>1.973234146519345</v>
+        <v>3.630549955459702</v>
       </c>
     </row>
     <row r="55">
@@ -2394,34 +2394,34 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>frozenset({'trillion', 'relief'})</t>
+          <t>frozenset({'senat', 'relief'})</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>frozenset({'senat'})</t>
+          <t>frozenset({'trillion'})</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.006563833278634723</v>
+        <v>0.01148670823761076</v>
       </c>
       <c r="E55" t="n">
-        <v>0.02067607482769938</v>
+        <v>0.01017394158188382</v>
       </c>
       <c r="F55" t="n">
         <v>0.005251066622907778</v>
       </c>
       <c r="G55" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.4571428571428571</v>
       </c>
       <c r="H55" t="n">
-        <v>38.69206349206349</v>
+        <v>44.93271889400922</v>
       </c>
       <c r="I55" t="n">
-        <v>0.005115352314882183</v>
+        <v>0.005134201524330182</v>
       </c>
       <c r="J55" t="n">
-        <v>4.896619625861502</v>
+        <v>1.823363791822845</v>
       </c>
     </row>
     <row r="56">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>frozenset({'trillion', 'senat'})</t>
+          <t>frozenset({'senat', 'trillion'})</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2466,34 +2466,34 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>frozenset({'relief', 'senat'})</t>
+          <t>frozenset({'relief', 'trillion'})</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>frozenset({'trillion'})</t>
+          <t>frozenset({'senat'})</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.01148670823761076</v>
+        <v>0.006563833278634723</v>
       </c>
       <c r="E57" t="n">
-        <v>0.01017394158188382</v>
+        <v>0.02067607482769938</v>
       </c>
       <c r="F57" t="n">
         <v>0.005251066622907778</v>
       </c>
       <c r="G57" t="n">
-        <v>0.4571428571428571</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="H57" t="n">
-        <v>44.93271889400922</v>
+        <v>38.69206349206349</v>
       </c>
       <c r="I57" t="n">
-        <v>0.005134201524330182</v>
+        <v>0.005115352314882183</v>
       </c>
       <c r="J57" t="n">
-        <v>1.823363791822845</v>
+        <v>4.896619625861502</v>
       </c>
     </row>
     <row r="58">
@@ -2507,7 +2507,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>frozenset({'relief', 'senat'})</t>
+          <t>frozenset({'senat', 'relief'})</t>
         </is>
       </c>
       <c r="D58" t="n">

</xml_diff>